<commit_message>
Modified sharp sensor price
</commit_message>
<xml_diff>
--- a/HARDWARE/Docs/Components list.xlsx
+++ b/HARDWARE/Docs/Components list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coa7clj\workspace\Laser_Scanner\LaserScanner\HARDWARE\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A865B5-DC75-4677-80FD-6C6CBAED4422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E53E5E-DE8D-40B0-9495-6A767CA90FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Total price</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -197,10 +200,16 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -213,12 +222,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -502,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,7 +551,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="1">
-        <v>59.38</v>
+        <v>65.08</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -568,7 +571,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="1">
-        <v>65.08</v>
+        <v>45.77</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -658,105 +661,110 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10">
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12">
         <f>SUMPRODUCT(E2:E7,D2:D7)</f>
-        <v>297.84999999999997</v>
-      </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
+        <v>264.93</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="12" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="7">
         <v>30</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="7">
         <v>19.04</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="7">
         <f>SUM(D11:F12)</f>
         <v>49.04</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10">
         <f>D13+D8</f>
-        <v>346.89</v>
-      </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
+        <v>313.97000000000003</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:F10"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="D14:F14"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="A12:C12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{D265F9ED-B4F3-4888-ADDE-C71BEF74BE79}"/>

</xml_diff>

<commit_message>
ordered some componenets and modified shopping list
</commit_message>
<xml_diff>
--- a/HARDWARE/Docs/Components list.xlsx
+++ b/HARDWARE/Docs/Components list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coa7clj\workspace\Laser_Scanner\LaserScanner\HARDWARE\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LaserScanner\LaserScanner\HARDWARE\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A865B5-DC75-4677-80FD-6C6CBAED4422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85CE67E-DBDE-4607-B779-9839CECC88BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Suplier</t>
   </si>
   <si>
-    <t>Farnell</t>
-  </si>
-  <si>
     <t>Ardushop</t>
   </si>
   <si>
@@ -124,6 +121,27 @@
   </si>
   <si>
     <t>Total price</t>
+  </si>
+  <si>
+    <t>29,95</t>
+  </si>
+  <si>
+    <t>Optimus Digital</t>
+  </si>
+  <si>
+    <t>PH2.0 Socket 3p</t>
+  </si>
+  <si>
+    <t>socket</t>
+  </si>
+  <si>
+    <t>3p PH2.00 Single Head Cable (20 cm)</t>
+  </si>
+  <si>
+    <t>WireSocket</t>
+  </si>
+  <si>
+    <t>Ordered</t>
   </si>
 </sst>
 </file>
@@ -133,7 +151,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$RON]\ #,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +166,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -237,6 +260,579 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>259080</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>152400</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>190500</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Check Box 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>160020</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>198120</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Check Box 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>259080</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>167640</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>190500</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>15240</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1027" name="Check Box 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1027"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>167640</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>198120</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>15240</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1028" name="Check Box 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1028"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>152400</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>198120</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1029" name="Check Box 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1029"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>144780</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>198120</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1030" name="Check Box 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1030"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>152400</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>198120</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1031" name="Check Box 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1031"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>274320</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>175260</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>205740</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>22860</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1032" name="Check Box 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1032"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -501,23 +1097,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -536,8 +1133,11 @@
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -547,8 +1147,8 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
-        <v>59.38</v>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -557,7 +1157,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -577,7 +1177,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -597,7 +1197,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -617,7 +1217,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -637,7 +1237,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -645,118 +1245,158 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1">
-        <v>28.27</v>
+        <v>0.99</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1">
+        <v>28.27</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10">
-        <f>SUMPRODUCT(E2:E7,D2:D7)</f>
-        <v>297.84999999999997</v>
-      </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10">
+        <f>SUMPRODUCT(E2:E9,D2:D9)</f>
+        <v>239.95000000000002</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="12" t="s">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8">
-        <v>19.04</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="8">
-        <f>SUM(D11:F12)</f>
-        <v>49.04</v>
+        <v>13.99</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14">
-        <f>D13+D8</f>
-        <v>346.89</v>
-      </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8">
+        <v>19.04</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8">
+        <f>SUM(D13:F14)</f>
+        <v>33.03</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="14">
+        <f>D15+D10</f>
+        <v>272.98</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:F16"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A9:F9"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="D10:F10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="A11:F11"/>
     <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D14:F14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{D265F9ED-B4F3-4888-ADDE-C71BEF74BE79}"/>
@@ -764,9 +1404,195 @@
     <hyperlink ref="F4" r:id="rId3" xr:uid="{E583D95D-E5A5-4C11-9754-B786E1B46291}"/>
     <hyperlink ref="F5" r:id="rId4" xr:uid="{4CDAAA45-F5D7-480F-881D-7E6DA03EC8C2}"/>
     <hyperlink ref="F6" r:id="rId5" xr:uid="{891CCC3F-847B-4C96-8024-BC63BF3D3D17}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{A9E592B7-FBCA-4E75-9DEA-86BB4A93AE65}"/>
+    <hyperlink ref="F9" r:id="rId6" xr:uid="{A9E592B7-FBCA-4E75-9DEA-86BB4A93AE65}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{AFD60E0B-8D6E-4C31-A177-6157977B8340}"/>
+    <hyperlink ref="F7" r:id="rId8" xr:uid="{92878A8E-A357-4930-940E-9ED67B5BF9BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <drawing r:id="rId10"/>
+  <legacyDrawing r:id="rId11"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1025" r:id="rId12" name="Check Box 1">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>259080</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>152400</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>190500</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1026" r:id="rId13" name="Check Box 2">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>160020</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>7620</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1027" r:id="rId14" name="Check Box 3">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>259080</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>167640</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>190500</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1028" r:id="rId15" name="Check Box 4">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>167640</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1029" r:id="rId16" name="Check Box 5">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>152400</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>7620</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1030" r:id="rId17" name="Check Box 6">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>144780</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>7620</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1031" r:id="rId18" name="Check Box 7">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>152400</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>7620</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1032" r:id="rId19" name="Check Box 8">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>274320</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>175260</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>205740</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>22860</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>